<commit_message>
Nuevos modulos de node JS
</commit_message>
<xml_diff>
--- a/campania/campania.xlsx
+++ b/campania/campania.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josema\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josema\Desktop\coderhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE633631-36C6-49B6-BE72-5BF9A32EE167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE4311D-8376-4133-B5FB-9643683A99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Campaña Santa Rosa" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>